<commit_message>
Practice Task N8 complete
</commit_message>
<xml_diff>
--- a/IBtask8/WorkAround/НоменклатураСЦенами.xlsx
+++ b/IBtask8/WorkAround/НоменклатураСЦенами.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t xml:space="preserve">Лопата</t>
   </si>
@@ -61,6 +61,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -142,16 +143,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -216,6 +217,14 @@
       </c>
       <c r="B8" s="0" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>786</v>
       </c>
     </row>
   </sheetData>

</xml_diff>